<commit_message>
Realizado 6.1 "Situación 1"
</commit_message>
<xml_diff>
--- a/RepartoTG2.xlsx
+++ b/RepartoTG2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cheda\Documents\Cheda\Sistemas de Información\3º SISTEMAS DE INFORMACIÓN\SEGUNDO CUATRIMESTRE\DTE\LAB\TG2_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FDFF04-832E-4618-A057-D1299E261023}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7295E7-316E-40C0-BBDC-E243D5D663D5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>1) Autores, planificación, entrega</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>José, Fernando Criterios E y F</t>
+  </si>
+  <si>
+    <t>Todos</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <dimension ref="C3:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +502,9 @@
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">

</xml_diff>

<commit_message>
Correcciones, añadido datos excel
</commit_message>
<xml_diff>
--- a/RepartoTG2.xlsx
+++ b/RepartoTG2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Urbano\Documents\GitHub\TG2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27519FE-C41F-4EDB-9F06-AABF2D708F53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>1) Autores, planificación, entrega</t>
   </si>
@@ -79,12 +85,15 @@
   </si>
   <si>
     <t>Fernando</t>
+  </si>
+  <si>
+    <t>Alberto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,27 +424,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="31.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.125" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +452,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -451,7 +460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -459,7 +468,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
@@ -467,7 +476,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
@@ -475,13 +484,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
@@ -489,7 +498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
@@ -497,7 +506,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
@@ -505,13 +514,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
@@ -519,11 +528,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>